<commit_message>
24-09-2020 commit for Python Automation project AIQCA
</commit_message>
<xml_diff>
--- a/Resources/configurations/testdata/Test_data.xlsx
+++ b/Resources/configurations/testdata/Test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumanth\PycharmProjects\PythonTesting\Resources\configurations\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{976614BF-7111-4F2F-8B5D-91C6AFB310EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE58A90-35F0-424E-AE30-D8316F8C6F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CA" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="143">
   <si>
     <t>External links</t>
   </si>
@@ -549,10 +549,100 @@
     <t>Config Advisorrrrrrrrrrrr</t>
   </si>
   <si>
-    <t>Objective: ONTAP Post Deployment Guided</t>
-  </si>
-  <si>
-    <t>Expert</t>
+    <t>test_cp_1_logo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Area </t>
+  </si>
+  <si>
+    <t>test_logo</t>
+  </si>
+  <si>
+    <t>TestCases</t>
+  </si>
+  <si>
+    <t>test_cp_2_NetApp_ActiveIQ</t>
+  </si>
+  <si>
+    <t>test_header_english</t>
+  </si>
+  <si>
+    <t>test_cp_3_Ative_IQ_Config_Advisor</t>
+  </si>
+  <si>
+    <t>test_cp_3_help_english</t>
+  </si>
+  <si>
+    <t>test_cp_3_notifications_english</t>
+  </si>
+  <si>
+    <t>test_cp_3_settings_english</t>
+  </si>
+  <si>
+    <t>test_cp_3_shutdown_english</t>
+  </si>
+  <si>
+    <t>Checkpoints with numbers</t>
+  </si>
+  <si>
+    <t>test_cp_4_ONTAP</t>
+  </si>
+  <si>
+    <t>test_cp_4_dashboard_english</t>
+  </si>
+  <si>
+    <t>test_cp_4_help_english</t>
+  </si>
+  <si>
+    <t>test_cp_4_notifications_english</t>
+  </si>
+  <si>
+    <t>test_cp_4_ontap_deploy_expert_english</t>
+  </si>
+  <si>
+    <t>test_cp_4_ontap_deploy_guided_english</t>
+  </si>
+  <si>
+    <t>test_cp_5_NetAppHCI</t>
+  </si>
+  <si>
+    <t>test_cp_5_dashboard_english</t>
+  </si>
+  <si>
+    <t>test_cp_5_help_english</t>
+  </si>
+  <si>
+    <t>test_cp_5_notifications_english</t>
+  </si>
+  <si>
+    <t>test_cp_6_MetroCluster</t>
+  </si>
+  <si>
+    <t>test_cp_6_dashboard_english</t>
+  </si>
+  <si>
+    <t>test_cp_6_help_english</t>
+  </si>
+  <si>
+    <t>test_cp_6_notifications_english</t>
+  </si>
+  <si>
+    <t>test_cp_7_NetAppSupportSite</t>
+  </si>
+  <si>
+    <t>test_cp_7_notifications_english</t>
+  </si>
+  <si>
+    <t>test_cp_8_notifications_english</t>
+  </si>
+  <si>
+    <t>test_cp_8_TrainingLink</t>
+  </si>
+  <si>
+    <t>test_cp_9_notifications_english</t>
+  </si>
+  <si>
+    <t>test_cp_9_TechnicalOverviewLink</t>
   </si>
 </sst>
 </file>
@@ -595,7 +685,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -626,8 +716,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -676,11 +772,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -690,14 +823,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -715,9 +846,6 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -736,6 +864,54 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1183,7 +1359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D092D5-FFEB-401F-A5DD-519D93C72D8B}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1201,13 +1377,13 @@
       <c r="A1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>51</v>
       </c>
       <c r="E1" s="3" t="s">
@@ -1218,7 +1394,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1238,7 +1414,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="18" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -1251,13 +1427,13 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+    <row r="4" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1271,7 +1447,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -1285,7 +1461,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1299,7 +1475,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1313,7 +1489,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -1327,7 +1503,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -1341,7 +1517,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1355,7 +1531,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -1369,7 +1545,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1383,7 +1559,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1396,13 +1572,13 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
+    <row r="15" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="16" t="s">
         <v>101</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -1416,7 +1592,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="16" t="s">
         <v>106</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1430,7 +1606,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="16" t="s">
         <v>106</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1444,7 +1620,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="16" t="s">
         <v>106</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -1458,7 +1634,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="16" t="s">
         <v>107</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -1472,7 +1648,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="19" t="s">
+      <c r="A21" s="16" t="s">
         <v>107</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -1486,8 +1662,8 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="19"/>
-      <c r="B22" s="20"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1497,17 +1673,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3A5B8E-108A-4858-82ED-4A6B4CF60D98}">
-  <dimension ref="A7:M41"/>
+  <dimension ref="A7:M60"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="10.109375" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
@@ -1520,379 +1696,631 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="5" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>5</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>5</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="7">
         <v>5</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>4</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="8">
         <v>18</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="8">
         <v>9</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="8">
         <v>5</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>6</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="9">
         <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B13" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
+      <c r="A14" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="7">
+      <c r="B14" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
+      <c r="A18" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="8" t="s">
+      <c r="A21" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="8" t="s">
+      <c r="A23" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="7">
+      <c r="B23" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="8" t="s">
+      <c r="A24" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="8" t="s">
+      <c r="A25" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="7">
+      <c r="B25" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
+      <c r="A26" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="B28" s="7">
+      <c r="B28" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="A30" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="5">
         <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="16"/>
+      <c r="A34" s="23"/>
       <c r="B34"/>
     </row>
     <row r="35" spans="1:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="23"/>
-      <c r="D35" s="22" t="s">
+      <c r="C35" s="20"/>
+      <c r="D35" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="23"/>
-      <c r="F35" s="22" t="s">
+      <c r="E35" s="20"/>
+      <c r="F35" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="G35" s="23"/>
-      <c r="H35" s="22" t="s">
+      <c r="G35" s="20"/>
+      <c r="H35" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="I35" s="23"/>
-      <c r="J35" s="22" t="s">
+      <c r="I35" s="20"/>
+      <c r="J35" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="K35" s="23"/>
-      <c r="L35" s="22" t="s">
+      <c r="K35" s="20"/>
+      <c r="L35" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="M35" s="23"/>
+      <c r="M35" s="20"/>
     </row>
     <row r="36" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="C36" s="17" t="s">
+      <c r="C36" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="G36" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="H36" s="17" t="s">
+      <c r="H36" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="I36" s="17" t="s">
+      <c r="I36" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="J36" s="17" t="s">
+      <c r="J36" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="K36" s="17" t="s">
+      <c r="K36" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="L36" s="17" t="s">
+      <c r="L36" s="14" t="s">
         <v>93</v>
       </c>
-      <c r="M36" s="17" t="s">
+      <c r="M36" s="14" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="17">
+      <c r="B37" s="14">
         <v>3</v>
       </c>
-      <c r="C37" s="17">
+      <c r="C37" s="14">
         <v>3</v>
       </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17">
+      <c r="D37" s="14">
         <v>2</v>
       </c>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17">
+      <c r="E37" s="14">
+        <v>2</v>
+      </c>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14">
         <v>3</v>
       </c>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17">
+      <c r="H37" s="14"/>
+      <c r="I37" s="14">
         <v>3</v>
       </c>
-      <c r="J37" s="17"/>
-      <c r="K37" s="17">
+      <c r="J37" s="14"/>
+      <c r="K37" s="14">
         <v>4</v>
       </c>
-      <c r="L37" s="17"/>
-      <c r="M37" s="17">
+      <c r="L37" s="14"/>
+      <c r="M37" s="14">
         <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17">
+      <c r="B38" s="14"/>
+      <c r="C38" s="14">
         <v>6</v>
       </c>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17">
+      <c r="D38" s="14">
+        <v>14</v>
+      </c>
+      <c r="E38" s="14">
         <v>6</v>
       </c>
-      <c r="F38" s="17"/>
-      <c r="G38" s="17">
+      <c r="F38" s="14"/>
+      <c r="G38" s="14">
         <v>7</v>
       </c>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17">
+      <c r="H38" s="14"/>
+      <c r="I38" s="14">
         <v>3</v>
       </c>
-      <c r="J38" s="17"/>
-      <c r="K38" s="17">
+      <c r="J38" s="14"/>
+      <c r="K38" s="14">
         <v>4</v>
       </c>
-      <c r="L38" s="17"/>
-      <c r="M38" s="17">
+      <c r="L38" s="14"/>
+      <c r="M38" s="14">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="28" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>112</v>
+      <c r="B41" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41" s="29">
+        <v>1</v>
+      </c>
+      <c r="D41" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A42" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42" s="28" t="s">
+        <v>116</v>
+      </c>
+      <c r="C42" s="29">
+        <v>2</v>
+      </c>
+      <c r="D42" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="B43" s="28" t="s">
+        <v>118</v>
+      </c>
+      <c r="C43" s="29">
+        <v>3</v>
+      </c>
+      <c r="D43" s="31">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="30"/>
+      <c r="B44" s="28" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="29">
+        <v>11</v>
+      </c>
+      <c r="D44" s="31"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A45" s="30"/>
+      <c r="B45" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" s="29">
+        <v>1</v>
+      </c>
+      <c r="D45" s="31"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" s="30"/>
+      <c r="B46" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C46" s="29">
+        <v>2</v>
+      </c>
+      <c r="D46" s="31"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B47" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C47" s="29">
+        <v>1</v>
+      </c>
+      <c r="D47" s="31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" s="30"/>
+      <c r="B48" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" s="29">
+        <v>2</v>
+      </c>
+      <c r="D48" s="31"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="30"/>
+      <c r="B49" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="C49" s="29">
+        <v>3</v>
+      </c>
+      <c r="D49" s="31"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="30"/>
+      <c r="B50" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="29">
+        <v>2</v>
+      </c>
+      <c r="D50" s="31"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="30"/>
+      <c r="B51" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" s="29">
+        <v>2</v>
+      </c>
+      <c r="D51" s="31"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="C52" s="29">
+        <v>1</v>
+      </c>
+      <c r="D52" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="30"/>
+      <c r="B53" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C53" s="29">
+        <v>1</v>
+      </c>
+      <c r="D53" s="31"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="30"/>
+      <c r="B54" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="29">
+        <v>2</v>
+      </c>
+      <c r="D54" s="31"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="33" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="C55" s="29">
+        <v>1</v>
+      </c>
+      <c r="D55" s="31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="34"/>
+      <c r="B56" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C56" s="29">
+        <v>1</v>
+      </c>
+      <c r="D56" s="31"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="35"/>
+      <c r="B57" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="29">
+        <v>2</v>
+      </c>
+      <c r="D57" s="31"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="32" t="s">
+        <v>137</v>
+      </c>
+      <c r="B58" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="C58" s="36">
+        <v>2</v>
+      </c>
+      <c r="D58" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" s="28" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="36">
+        <v>2</v>
+      </c>
+      <c r="D59" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B60" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="C60" s="36">
+        <v>2</v>
+      </c>
+      <c r="D60" s="29">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="14">
+    <mergeCell ref="D52:D54"/>
+    <mergeCell ref="A52:A54"/>
+    <mergeCell ref="D55:D57"/>
+    <mergeCell ref="A55:A57"/>
+    <mergeCell ref="D43:D46"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="D47:D51"/>
+    <mergeCell ref="A47:A51"/>
     <mergeCell ref="L35:M35"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="D35:E35"/>

</xml_diff>

<commit_message>
05-10-2020 commit for Python Automation project AIQCA - END of Local commit
</commit_message>
<xml_diff>
--- a/Resources/configurations/testdata/Test_data.xlsx
+++ b/Resources/configurations/testdata/Test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sumanth\PycharmProjects\PythonTesting\Resources\configurations\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AE58A90-35F0-424E-AE30-D8316F8C6F15}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46E5ED57-9F9E-4C9D-9D9F-0266223CE0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CA" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="147">
   <si>
     <t>External links</t>
   </si>
@@ -644,6 +644,18 @@
   <si>
     <t>test_cp_9_TechnicalOverviewLink</t>
   </si>
+  <si>
+    <t>test_cp_10_whats_new</t>
+  </si>
+  <si>
+    <t>test_cp_11_Demo_Video</t>
+  </si>
+  <si>
+    <t>test_cp_10_help_english</t>
+  </si>
+  <si>
+    <t>test_cp_11_help_english</t>
+  </si>
 </sst>
 </file>
 
@@ -685,7 +697,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -719,6 +731,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -813,7 +831,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -859,58 +877,67 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1359,7 +1386,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18D092D5-FFEB-401F-A5DD-519D93C72D8B}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1673,15 +1700,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3A5B8E-108A-4858-82ED-4A6B4CF60D98}">
-  <dimension ref="A7:M60"/>
+  <dimension ref="A7:M62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="33.6640625" style="23" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" style="4" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
@@ -1696,7 +1723,7 @@
   </cols>
   <sheetData>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="19" t="s">
         <v>73</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -1716,7 +1743,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="19" t="s">
         <v>53</v>
       </c>
       <c r="B8" s="7">
@@ -1736,7 +1763,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="19" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="8">
@@ -1756,7 +1783,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="19" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -1764,7 +1791,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="20" t="s">
         <v>48</v>
       </c>
       <c r="B12" s="6">
@@ -1772,7 +1799,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="20" t="s">
         <v>55</v>
       </c>
       <c r="B13" s="6">
@@ -1780,7 +1807,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="20" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="6">
@@ -1788,7 +1815,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="20" t="s">
         <v>56</v>
       </c>
       <c r="B15" s="6">
@@ -1796,7 +1823,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B16" s="6">
@@ -1804,7 +1831,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="22" t="s">
+      <c r="A17" s="20" t="s">
         <v>58</v>
       </c>
       <c r="B17" s="6">
@@ -1812,7 +1839,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="20" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="6">
@@ -1820,7 +1847,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="20" t="s">
         <v>59</v>
       </c>
       <c r="B19" s="6">
@@ -1828,7 +1855,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="22" t="s">
+      <c r="A20" s="20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="6">
@@ -1836,7 +1863,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="20" t="s">
         <v>60</v>
       </c>
       <c r="B21" s="6">
@@ -1844,7 +1871,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="20" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="6">
@@ -1852,7 +1879,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="6">
@@ -1860,7 +1887,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="22" t="s">
+      <c r="A24" s="20" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="6">
@@ -1868,7 +1895,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="22" t="s">
+      <c r="A25" s="20" t="s">
         <v>61</v>
       </c>
       <c r="B25" s="6">
@@ -1876,7 +1903,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="22" t="s">
+      <c r="A26" s="20" t="s">
         <v>62</v>
       </c>
       <c r="B26" s="6">
@@ -1884,7 +1911,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="20" t="s">
         <v>63</v>
       </c>
       <c r="B27" s="6">
@@ -1892,7 +1919,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="22" t="s">
+      <c r="A28" s="20" t="s">
         <v>64</v>
       </c>
       <c r="B28" s="6">
@@ -1900,7 +1927,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="20" t="s">
         <v>65</v>
       </c>
       <c r="B29" s="6">
@@ -1908,7 +1935,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="22" t="s">
+      <c r="A30" s="20" t="s">
         <v>66</v>
       </c>
       <c r="B30" s="6">
@@ -1916,7 +1943,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
+      <c r="A31" s="19" t="s">
         <v>67</v>
       </c>
       <c r="B31" s="5">
@@ -1924,40 +1951,40 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="23"/>
+      <c r="A34" s="21"/>
       <c r="B34"/>
     </row>
     <row r="35" spans="1:13" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="24" t="s">
+      <c r="A35" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="19" t="s">
+      <c r="C35" s="36"/>
+      <c r="D35" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="19" t="s">
+      <c r="E35" s="36"/>
+      <c r="F35" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="G35" s="20"/>
-      <c r="H35" s="19" t="s">
+      <c r="G35" s="36"/>
+      <c r="H35" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="I35" s="20"/>
-      <c r="J35" s="19" t="s">
+      <c r="I35" s="36"/>
+      <c r="J35" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="K35" s="20"/>
-      <c r="L35" s="19" t="s">
+      <c r="K35" s="36"/>
+      <c r="L35" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="M35" s="20"/>
+      <c r="M35" s="36"/>
     </row>
     <row r="36" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="22" t="s">
         <v>92</v>
       </c>
       <c r="B36" s="14" t="s">
@@ -1998,7 +2025,7 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="22" t="s">
         <v>94</v>
       </c>
       <c r="B37" s="14">
@@ -2013,11 +2040,15 @@
       <c r="E37" s="14">
         <v>2</v>
       </c>
-      <c r="F37" s="14"/>
+      <c r="F37" s="14">
+        <v>2</v>
+      </c>
       <c r="G37" s="14">
         <v>3</v>
       </c>
-      <c r="H37" s="14"/>
+      <c r="H37" s="14">
+        <v>4</v>
+      </c>
       <c r="I37" s="14">
         <v>3</v>
       </c>
@@ -2031,7 +2062,7 @@
       </c>
     </row>
     <row r="38" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="22" t="s">
         <v>95</v>
       </c>
       <c r="B38" s="14"/>
@@ -2044,11 +2075,15 @@
       <c r="E38" s="14">
         <v>6</v>
       </c>
-      <c r="F38" s="14"/>
+      <c r="F38" s="14">
+        <v>6</v>
+      </c>
       <c r="G38" s="14">
         <v>7</v>
       </c>
-      <c r="H38" s="14"/>
+      <c r="H38" s="14">
+        <v>10</v>
+      </c>
       <c r="I38" s="14">
         <v>3</v>
       </c>
@@ -2062,257 +2097,291 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A40" s="26" t="s">
+      <c r="A40" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="27" t="s">
+      <c r="B40" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="D40" s="27" t="s">
+      <c r="D40" s="25" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A41" s="28" t="s">
+      <c r="A41" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B41" s="28" t="s">
+      <c r="B41" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="29">
+      <c r="C41" s="27">
         <v>1</v>
       </c>
-      <c r="D41" s="29">
+      <c r="D41" s="27">
         <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A42" s="28" t="s">
+      <c r="A42" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="C42" s="29">
+      <c r="C42" s="27">
         <v>2</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D42" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A43" s="30" t="s">
+      <c r="A43" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="B43" s="28" t="s">
+      <c r="B43" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="C43" s="29">
+      <c r="C43" s="27">
         <v>3</v>
       </c>
-      <c r="D43" s="31">
+      <c r="D43" s="30">
         <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A44" s="30"/>
-      <c r="B44" s="28" t="s">
+      <c r="A44" s="31"/>
+      <c r="B44" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="C44" s="29">
+      <c r="C44" s="27">
         <v>11</v>
       </c>
-      <c r="D44" s="31"/>
+      <c r="D44" s="30"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A45" s="30"/>
-      <c r="B45" s="28" t="s">
+      <c r="A45" s="31"/>
+      <c r="B45" s="26" t="s">
         <v>120</v>
       </c>
-      <c r="C45" s="29">
+      <c r="C45" s="27">
         <v>1</v>
       </c>
-      <c r="D45" s="31"/>
+      <c r="D45" s="30"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A46" s="30"/>
-      <c r="B46" s="28" t="s">
+      <c r="A46" s="31"/>
+      <c r="B46" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="C46" s="29">
+      <c r="C46" s="27">
         <v>2</v>
       </c>
-      <c r="D46" s="31"/>
+      <c r="D46" s="30"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="B47" s="28" t="s">
+      <c r="B47" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="C47" s="29">
+      <c r="C47" s="27">
         <v>1</v>
       </c>
-      <c r="D47" s="31">
+      <c r="D47" s="30">
         <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A48" s="30"/>
-      <c r="B48" s="28" t="s">
+      <c r="A48" s="31"/>
+      <c r="B48" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C48" s="29">
+      <c r="C48" s="27">
         <v>2</v>
       </c>
-      <c r="D48" s="31"/>
+      <c r="D48" s="30"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" s="30"/>
-      <c r="B49" s="28" t="s">
+      <c r="A49" s="31"/>
+      <c r="B49" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="C49" s="29">
+      <c r="C49" s="27">
         <v>3</v>
       </c>
-      <c r="D49" s="31"/>
+      <c r="D49" s="30"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="30"/>
-      <c r="B50" s="28" t="s">
+      <c r="A50" s="31"/>
+      <c r="B50" s="26" t="s">
         <v>127</v>
       </c>
-      <c r="C50" s="29">
+      <c r="C50" s="27">
         <v>2</v>
       </c>
-      <c r="D50" s="31"/>
+      <c r="D50" s="30"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" s="30"/>
-      <c r="B51" s="28" t="s">
+      <c r="A51" s="31"/>
+      <c r="B51" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="C51" s="29">
+      <c r="C51" s="27">
         <v>2</v>
       </c>
-      <c r="D51" s="31"/>
+      <c r="D51" s="30"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="31" t="s">
         <v>129</v>
       </c>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="26" t="s">
         <v>130</v>
       </c>
-      <c r="C52" s="29">
+      <c r="C52" s="27">
         <v>1</v>
       </c>
-      <c r="D52" s="31">
+      <c r="D52" s="30">
         <v>4</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="30"/>
-      <c r="B53" s="28" t="s">
+      <c r="A53" s="31"/>
+      <c r="B53" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="C53" s="29">
+      <c r="C53" s="27">
         <v>1</v>
       </c>
-      <c r="D53" s="31"/>
+      <c r="D53" s="30"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="30"/>
-      <c r="B54" s="28" t="s">
+      <c r="A54" s="31"/>
+      <c r="B54" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="C54" s="29">
+      <c r="C54" s="27">
         <v>2</v>
       </c>
-      <c r="D54" s="31"/>
+      <c r="D54" s="30"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="33" t="s">
+      <c r="A55" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="B55" s="28" t="s">
+      <c r="B55" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="C55" s="29">
+      <c r="C55" s="27">
         <v>1</v>
       </c>
-      <c r="D55" s="31">
+      <c r="D55" s="30">
         <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="34"/>
-      <c r="B56" s="28" t="s">
+      <c r="A56" s="33"/>
+      <c r="B56" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="C56" s="29">
+      <c r="C56" s="27">
         <v>1</v>
       </c>
-      <c r="D56" s="31"/>
+      <c r="D56" s="30"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="35"/>
-      <c r="B57" s="28" t="s">
+      <c r="A57" s="34"/>
+      <c r="B57" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="C57" s="29">
+      <c r="C57" s="27">
         <v>2</v>
       </c>
-      <c r="D57" s="31"/>
+      <c r="D57" s="30"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="32" t="s">
+      <c r="A58" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="C58" s="36">
+      <c r="C58" s="29">
         <v>2</v>
       </c>
-      <c r="D58" s="29">
+      <c r="D58" s="27">
         <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="32" t="s">
+      <c r="A59" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="B59" s="28" t="s">
+      <c r="B59" s="38" t="s">
         <v>139</v>
       </c>
-      <c r="C59" s="36">
+      <c r="C59" s="39">
         <v>2</v>
       </c>
-      <c r="D59" s="29">
+      <c r="D59" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="32" t="s">
+      <c r="A60" s="37" t="s">
         <v>142</v>
       </c>
-      <c r="B60" s="28" t="s">
+      <c r="B60" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="C60" s="36">
+      <c r="C60" s="39">
         <v>2</v>
       </c>
-      <c r="D60" s="29">
+      <c r="D60" s="39">
         <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="B61" s="37" t="s">
+        <v>145</v>
+      </c>
+      <c r="C61" s="39">
+        <v>3</v>
+      </c>
+      <c r="D61" s="39">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C62" s="39">
+        <v>3</v>
+      </c>
+      <c r="D62" s="39">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="L35:M35"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="J35:K35"/>
     <mergeCell ref="D52:D54"/>
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="D55:D57"/>
@@ -2321,12 +2390,6 @@
     <mergeCell ref="A43:A46"/>
     <mergeCell ref="D47:D51"/>
     <mergeCell ref="A47:A51"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="J35:K35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>